<commit_message>
Update template to use named cells to help simplfy code
</commit_message>
<xml_diff>
--- a/PackListTemplate.xlsx
+++ b/PackListTemplate.xlsx
@@ -1,25 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20228"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmagnuson\OneDrive - tervis\Documents\WindowsPowerShell\Modules\TervisCustomizer\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0201B4-D696-40C1-A64E-F2A57E1220D9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="300" windowWidth="15600" windowHeight="11700" tabRatio="832"/>
+    <workbookView xWindow="480" yWindow="300" windowWidth="15600" windowHeight="11700" tabRatio="832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PackingList" sheetId="12" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="DataRange">PackingList!$A$16:$O$16</definedName>
     <definedName name="DownloadDate" localSheetId="0">PackingList!$L$4:$L$4</definedName>
     <definedName name="DownloadTime" localSheetId="0">PackingList!$L$5:$L$5</definedName>
+    <definedName name="FirstCellOfPacklistLineData" localSheetId="0">PackingList!$A$16</definedName>
+    <definedName name="GrandTotal" localSheetId="0">PackingList!$Q$12</definedName>
+    <definedName name="Total10WAV" localSheetId="0">PackingList!$Q$6</definedName>
+    <definedName name="Total16BEER" localSheetId="0">PackingList!$Q$9</definedName>
+    <definedName name="Total16DWT" localSheetId="0">PackingList!$Q$7</definedName>
+    <definedName name="Total16MUG" localSheetId="0">PackingList!$Q$8</definedName>
+    <definedName name="Total24DWT" localSheetId="0">PackingList!$Q$10</definedName>
+    <definedName name="Total24WB" localSheetId="0">PackingList!$Q$11</definedName>
+    <definedName name="Total6SIP" localSheetId="0">PackingList!$Q$3</definedName>
+    <definedName name="Total9SWG" localSheetId="0">PackingList!$Q$4</definedName>
+    <definedName name="Total9WINE" localSheetId="0">PackingList!$Q$5</definedName>
   </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>#</t>
   </si>
@@ -57,9 +73,6 @@
     <t>Download Time:</t>
   </si>
   <si>
-    <t>[Quantity]</t>
-  </si>
-  <si>
     <t>Batch</t>
   </si>
   <si>
@@ -72,30 +85,12 @@
     <t>Size</t>
   </si>
   <si>
-    <t>[Size]</t>
-  </si>
-  <si>
-    <t>[Sum]</t>
-  </si>
-  <si>
-    <t>[Batch]</t>
-  </si>
-  <si>
     <t>Grand Total:</t>
   </si>
   <si>
     <t>Receipt</t>
   </si>
   <si>
-    <t>[SO]</t>
-  </si>
-  <si>
-    <t>[DesignNum]</t>
-  </si>
-  <si>
-    <t>[SchNumber]</t>
-  </si>
-  <si>
     <t>Total 10WAV:</t>
   </si>
   <si>
@@ -108,46 +103,19 @@
     <t>Total 24WB:</t>
   </si>
   <si>
-    <t>[Total10WAV]</t>
-  </si>
-  <si>
-    <t>[Total16DWT]</t>
-  </si>
-  <si>
-    <t>[Total24DWT]</t>
-  </si>
-  <si>
-    <t>[Total24WB]</t>
-  </si>
-  <si>
     <t>Total 9SWG:</t>
   </si>
   <si>
     <t>Total 9WINE:</t>
   </si>
   <si>
-    <t>[Total9SWG]</t>
-  </si>
-  <si>
-    <t>[Total9WINE]</t>
-  </si>
-  <si>
     <t xml:space="preserve">                       PO #:</t>
   </si>
   <si>
     <t>Total 6SIP:</t>
   </si>
   <si>
-    <t>[Total6SIP]</t>
-  </si>
-  <si>
     <t>Total 16MUG:</t>
-  </si>
-  <si>
-    <t>[Total16MUG]</t>
-  </si>
-  <si>
-    <t>[Total16BEER]</t>
   </si>
   <si>
     <t>Total 16BEER:</t>
@@ -156,11 +124,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="\ 0;\-0;;@"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -326,7 +294,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -361,7 +329,7 @@
         <xdr:cNvPr id="4" name="Picture 3" descr="\\tervis\creative\Marketing\Brand Resources\2017 Branding\2_Logos\1_Primary_Logo\CMYK\2017_V2_PrimaryLogo_(CMYK).jpg">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDD2510C-1209-4CB0-9694-F0AD10B09531}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CDD2510C-1209-4CB0-9694-F0AD10B09531}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -371,7 +339,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -442,7 +410,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -474,9 +442,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -508,6 +494,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -683,153 +687,153 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:Q16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q16" sqref="Q16"/>
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.88671875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="3.44140625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" style="2"/>
-    <col min="4" max="4" width="2.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.6640625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="2.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="2.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.88671875" style="7" customWidth="1"/>
-    <col min="10" max="10" width="2.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.109375" style="2"/>
-    <col min="12" max="12" width="4.44140625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="8.33203125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="3.88671875" style="2" customWidth="1"/>
-    <col min="15" max="15" width="7.33203125" style="2" customWidth="1"/>
-    <col min="16" max="16" width="13.5546875" style="2" customWidth="1"/>
-    <col min="17" max="17" width="14.44140625" style="2" customWidth="1"/>
-    <col min="18" max="16384" width="9.109375" style="2"/>
+    <col min="1" max="1" width="7.85546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="3.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="2"/>
+    <col min="4" max="4" width="2.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="2.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.7109375" style="2" customWidth="1"/>
+    <col min="8" max="8" width="2.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" style="7" customWidth="1"/>
+    <col min="10" max="10" width="2.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="2"/>
+    <col min="12" max="12" width="4.42578125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="8.28515625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="3.85546875" style="2" customWidth="1"/>
+    <col min="15" max="15" width="7.28515625" style="2" customWidth="1"/>
+    <col min="16" max="16" width="13.5703125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" style="2" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:17" ht="18">
+    <row r="2" spans="1:17" ht="18.75" x14ac:dyDescent="0.3">
       <c r="I2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:17" s="17" customFormat="1" ht="18">
+    <row r="3" spans="1:17" s="17" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="I3" s="1"/>
       <c r="K3" s="1"/>
       <c r="P3" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
+        <v>25</v>
+      </c>
+      <c r="Q3" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I4" s="22" t="s">
         <v>10</v>
       </c>
       <c r="J4" s="22"/>
       <c r="K4" s="22"/>
       <c r="L4" s="22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="M4" s="22"/>
       <c r="N4" s="22"/>
       <c r="P4" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q4" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
+        <v>22</v>
+      </c>
+      <c r="Q4" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I5" s="22" t="s">
         <v>11</v>
       </c>
       <c r="J5" s="22"/>
       <c r="K5" s="22"/>
       <c r="L5" s="22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M5" s="22"/>
       <c r="N5" s="22"/>
       <c r="P5" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q5" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
+        <v>23</v>
+      </c>
+      <c r="Q5" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I6" s="23" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="J6" s="23"/>
       <c r="K6" s="23"/>
       <c r="P6" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q6" s="6" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
+        <v>18</v>
+      </c>
+      <c r="Q6" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="P7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q7" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" s="18" customFormat="1">
+        <v>19</v>
+      </c>
+      <c r="Q7" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="I8" s="7"/>
       <c r="P8" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q8" s="6" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17">
+        <v>26</v>
+      </c>
+      <c r="Q8" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="P9" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q9" s="21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17">
+        <v>27</v>
+      </c>
+      <c r="Q9" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="P10" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q10" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" s="19" customFormat="1">
+        <v>20</v>
+      </c>
+      <c r="Q10" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" s="19" customFormat="1" x14ac:dyDescent="0.25">
       <c r="I11" s="7"/>
       <c r="P11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q11" s="6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17">
+        <v>21</v>
+      </c>
+      <c r="Q11" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="P12" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q12" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" s="10" customFormat="1">
+        <v>16</v>
+      </c>
+      <c r="Q12" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C13" s="10" t="s">
         <v>3</v>
@@ -838,7 +842,7 @@
         <v>4</v>
       </c>
       <c r="G13" s="10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I13" s="11" t="s">
         <v>5</v>
@@ -847,7 +851,7 @@
         <v>7</v>
       </c>
       <c r="M13" s="10" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="O13" s="10" t="s">
         <v>8</v>
@@ -856,7 +860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:17" s="12" customFormat="1">
+    <row r="14" spans="1:17" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C14" s="12" t="s">
         <v>0</v>
       </c>
@@ -882,7 +886,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:17" s="10" customFormat="1">
+    <row r="15" spans="1:17" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="14"/>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
@@ -900,25 +904,8 @@
       <c r="O15" s="14"/>
       <c r="P15" s="16"/>
     </row>
-    <row r="16" spans="1:17">
-      <c r="A16" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I16" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="P16" s="7" t="s">
-        <v>24</v>
-      </c>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P16" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
Add value to named cell as they don't show up in the api without values
</commit_message>
<xml_diff>
--- a/PackListTemplate.xlsx
+++ b/PackListTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmagnuson\OneDrive - tervis\Documents\WindowsPowerShell\Modules\TervisCustomizer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E0201B4-D696-40C1-A64E-F2A57E1220D9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75BD674D-A6E6-45C7-A7A5-79A55C22C130}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="300" windowWidth="15600" windowHeight="11700" tabRatio="832" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -691,7 +691,7 @@
   <dimension ref="A2:Q16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,6 +905,9 @@
       <c r="P15" s="16"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>0</v>
+      </c>
       <c r="P16" s="7"/>
     </row>
   </sheetData>

</xml_diff>